<commit_message>
cap 1 de levítico anotado
</commit_message>
<xml_diff>
--- a/books.xlsx
+++ b/books.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$P$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$Q$67</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$Q$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$1:$P$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$B$1:$O$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -1233,10 +1233,10 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
-      <selection pane="bottomRight" activeCell="Q4" activeCellId="0" sqref="Q4"/>
+      <selection pane="bottomRight" activeCell="Q5" activeCellId="0" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.77"/>
@@ -1467,7 +1467,9 @@
       <c r="P4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q4" s="4"/>
+      <c r="Q4" s="4" t="n">
+        <v>0.5</v>
+      </c>
       <c r="R4" s="4" t="s">
         <v>27</v>
       </c>
@@ -3583,9 +3585,6 @@
       <c r="P42" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="Q42" s="4" t="n">
-        <v>0.5</v>
-      </c>
       <c r="R42" s="4" t="s">
         <v>226</v>
       </c>
@@ -3640,7 +3639,9 @@
       <c r="P43" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="Q43" s="4"/>
+      <c r="Q43" s="4" t="n">
+        <v>0.5</v>
+      </c>
       <c r="R43" s="4" t="s">
         <v>226</v>
       </c>
@@ -4957,7 +4958,7 @@
       <c r="A71" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:P67"/>
+  <autoFilter ref="B1:Q67"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>